<commit_message>
make two rake file import data
</commit_message>
<xml_diff>
--- a/data/ortholog_group_naming_09052016.xlsx
+++ b/data/ortholog_group_naming_09052016.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuan/Desktop/WishartLab/orthology_db/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="44940" yWindow="-3140" windowWidth="22260" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="325">
   <si>
     <t>Group by year</t>
   </si>
@@ -972,12 +983,6 @@
     <t>11a5_1424</t>
   </si>
   <si>
-    <t>201 rdh genes</t>
-  </si>
-  <si>
-    <t>min 2, max 15 in groups</t>
-  </si>
-  <si>
     <t>dcmb_1428</t>
   </si>
   <si>
@@ -994,9 +999,6 @@
   </si>
   <si>
     <t>11a5_1404</t>
-  </si>
-  <si>
-    <t>55 groups</t>
   </si>
   <si>
     <t>IBK_1358</t>
@@ -1008,8 +1010,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,6 +1042,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1062,7 +1080,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1070,14 +1088,130 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1145,7 +1279,123 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="117">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1458,465 +1708,465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN241"/>
+  <dimension ref="A1:AN238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="D151" sqref="D151"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="A239" sqref="A239:F241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="10" customWidth="1"/>
     <col min="2" max="2" width="12" style="10"/>
-    <col min="3" max="3" width="16.453125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="23.5" style="10" customWidth="1"/>
     <col min="6" max="6" width="13" style="10" customWidth="1"/>
     <col min="7" max="256" width="12" style="10"/>
-    <col min="257" max="257" width="13.6328125" style="10" customWidth="1"/>
+    <col min="257" max="257" width="13.6640625" style="10" customWidth="1"/>
     <col min="258" max="258" width="12" style="10"/>
-    <col min="259" max="259" width="16.453125" style="10" customWidth="1"/>
-    <col min="260" max="260" width="18.90625" style="10" customWidth="1"/>
-    <col min="261" max="261" width="23.54296875" style="10" customWidth="1"/>
+    <col min="259" max="259" width="16.5" style="10" customWidth="1"/>
+    <col min="260" max="260" width="18.83203125" style="10" customWidth="1"/>
+    <col min="261" max="261" width="23.5" style="10" customWidth="1"/>
     <col min="262" max="262" width="13" style="10" customWidth="1"/>
     <col min="263" max="512" width="12" style="10"/>
-    <col min="513" max="513" width="13.6328125" style="10" customWidth="1"/>
+    <col min="513" max="513" width="13.6640625" style="10" customWidth="1"/>
     <col min="514" max="514" width="12" style="10"/>
-    <col min="515" max="515" width="16.453125" style="10" customWidth="1"/>
-    <col min="516" max="516" width="18.90625" style="10" customWidth="1"/>
-    <col min="517" max="517" width="23.54296875" style="10" customWidth="1"/>
+    <col min="515" max="515" width="16.5" style="10" customWidth="1"/>
+    <col min="516" max="516" width="18.83203125" style="10" customWidth="1"/>
+    <col min="517" max="517" width="23.5" style="10" customWidth="1"/>
     <col min="518" max="518" width="13" style="10" customWidth="1"/>
     <col min="519" max="768" width="12" style="10"/>
-    <col min="769" max="769" width="13.6328125" style="10" customWidth="1"/>
+    <col min="769" max="769" width="13.6640625" style="10" customWidth="1"/>
     <col min="770" max="770" width="12" style="10"/>
-    <col min="771" max="771" width="16.453125" style="10" customWidth="1"/>
-    <col min="772" max="772" width="18.90625" style="10" customWidth="1"/>
-    <col min="773" max="773" width="23.54296875" style="10" customWidth="1"/>
+    <col min="771" max="771" width="16.5" style="10" customWidth="1"/>
+    <col min="772" max="772" width="18.83203125" style="10" customWidth="1"/>
+    <col min="773" max="773" width="23.5" style="10" customWidth="1"/>
     <col min="774" max="774" width="13" style="10" customWidth="1"/>
     <col min="775" max="1024" width="12" style="10"/>
-    <col min="1025" max="1025" width="13.6328125" style="10" customWidth="1"/>
+    <col min="1025" max="1025" width="13.6640625" style="10" customWidth="1"/>
     <col min="1026" max="1026" width="12" style="10"/>
-    <col min="1027" max="1027" width="16.453125" style="10" customWidth="1"/>
-    <col min="1028" max="1028" width="18.90625" style="10" customWidth="1"/>
-    <col min="1029" max="1029" width="23.54296875" style="10" customWidth="1"/>
+    <col min="1027" max="1027" width="16.5" style="10" customWidth="1"/>
+    <col min="1028" max="1028" width="18.83203125" style="10" customWidth="1"/>
+    <col min="1029" max="1029" width="23.5" style="10" customWidth="1"/>
     <col min="1030" max="1030" width="13" style="10" customWidth="1"/>
     <col min="1031" max="1280" width="12" style="10"/>
-    <col min="1281" max="1281" width="13.6328125" style="10" customWidth="1"/>
+    <col min="1281" max="1281" width="13.6640625" style="10" customWidth="1"/>
     <col min="1282" max="1282" width="12" style="10"/>
-    <col min="1283" max="1283" width="16.453125" style="10" customWidth="1"/>
-    <col min="1284" max="1284" width="18.90625" style="10" customWidth="1"/>
-    <col min="1285" max="1285" width="23.54296875" style="10" customWidth="1"/>
+    <col min="1283" max="1283" width="16.5" style="10" customWidth="1"/>
+    <col min="1284" max="1284" width="18.83203125" style="10" customWidth="1"/>
+    <col min="1285" max="1285" width="23.5" style="10" customWidth="1"/>
     <col min="1286" max="1286" width="13" style="10" customWidth="1"/>
     <col min="1287" max="1536" width="12" style="10"/>
-    <col min="1537" max="1537" width="13.6328125" style="10" customWidth="1"/>
+    <col min="1537" max="1537" width="13.6640625" style="10" customWidth="1"/>
     <col min="1538" max="1538" width="12" style="10"/>
-    <col min="1539" max="1539" width="16.453125" style="10" customWidth="1"/>
-    <col min="1540" max="1540" width="18.90625" style="10" customWidth="1"/>
-    <col min="1541" max="1541" width="23.54296875" style="10" customWidth="1"/>
+    <col min="1539" max="1539" width="16.5" style="10" customWidth="1"/>
+    <col min="1540" max="1540" width="18.83203125" style="10" customWidth="1"/>
+    <col min="1541" max="1541" width="23.5" style="10" customWidth="1"/>
     <col min="1542" max="1542" width="13" style="10" customWidth="1"/>
     <col min="1543" max="1792" width="12" style="10"/>
-    <col min="1793" max="1793" width="13.6328125" style="10" customWidth="1"/>
+    <col min="1793" max="1793" width="13.6640625" style="10" customWidth="1"/>
     <col min="1794" max="1794" width="12" style="10"/>
-    <col min="1795" max="1795" width="16.453125" style="10" customWidth="1"/>
-    <col min="1796" max="1796" width="18.90625" style="10" customWidth="1"/>
-    <col min="1797" max="1797" width="23.54296875" style="10" customWidth="1"/>
+    <col min="1795" max="1795" width="16.5" style="10" customWidth="1"/>
+    <col min="1796" max="1796" width="18.83203125" style="10" customWidth="1"/>
+    <col min="1797" max="1797" width="23.5" style="10" customWidth="1"/>
     <col min="1798" max="1798" width="13" style="10" customWidth="1"/>
     <col min="1799" max="2048" width="12" style="10"/>
-    <col min="2049" max="2049" width="13.6328125" style="10" customWidth="1"/>
+    <col min="2049" max="2049" width="13.6640625" style="10" customWidth="1"/>
     <col min="2050" max="2050" width="12" style="10"/>
-    <col min="2051" max="2051" width="16.453125" style="10" customWidth="1"/>
-    <col min="2052" max="2052" width="18.90625" style="10" customWidth="1"/>
-    <col min="2053" max="2053" width="23.54296875" style="10" customWidth="1"/>
+    <col min="2051" max="2051" width="16.5" style="10" customWidth="1"/>
+    <col min="2052" max="2052" width="18.83203125" style="10" customWidth="1"/>
+    <col min="2053" max="2053" width="23.5" style="10" customWidth="1"/>
     <col min="2054" max="2054" width="13" style="10" customWidth="1"/>
     <col min="2055" max="2304" width="12" style="10"/>
-    <col min="2305" max="2305" width="13.6328125" style="10" customWidth="1"/>
+    <col min="2305" max="2305" width="13.6640625" style="10" customWidth="1"/>
     <col min="2306" max="2306" width="12" style="10"/>
-    <col min="2307" max="2307" width="16.453125" style="10" customWidth="1"/>
-    <col min="2308" max="2308" width="18.90625" style="10" customWidth="1"/>
-    <col min="2309" max="2309" width="23.54296875" style="10" customWidth="1"/>
+    <col min="2307" max="2307" width="16.5" style="10" customWidth="1"/>
+    <col min="2308" max="2308" width="18.83203125" style="10" customWidth="1"/>
+    <col min="2309" max="2309" width="23.5" style="10" customWidth="1"/>
     <col min="2310" max="2310" width="13" style="10" customWidth="1"/>
     <col min="2311" max="2560" width="12" style="10"/>
-    <col min="2561" max="2561" width="13.6328125" style="10" customWidth="1"/>
+    <col min="2561" max="2561" width="13.6640625" style="10" customWidth="1"/>
     <col min="2562" max="2562" width="12" style="10"/>
-    <col min="2563" max="2563" width="16.453125" style="10" customWidth="1"/>
-    <col min="2564" max="2564" width="18.90625" style="10" customWidth="1"/>
-    <col min="2565" max="2565" width="23.54296875" style="10" customWidth="1"/>
+    <col min="2563" max="2563" width="16.5" style="10" customWidth="1"/>
+    <col min="2564" max="2564" width="18.83203125" style="10" customWidth="1"/>
+    <col min="2565" max="2565" width="23.5" style="10" customWidth="1"/>
     <col min="2566" max="2566" width="13" style="10" customWidth="1"/>
     <col min="2567" max="2816" width="12" style="10"/>
-    <col min="2817" max="2817" width="13.6328125" style="10" customWidth="1"/>
+    <col min="2817" max="2817" width="13.6640625" style="10" customWidth="1"/>
     <col min="2818" max="2818" width="12" style="10"/>
-    <col min="2819" max="2819" width="16.453125" style="10" customWidth="1"/>
-    <col min="2820" max="2820" width="18.90625" style="10" customWidth="1"/>
-    <col min="2821" max="2821" width="23.54296875" style="10" customWidth="1"/>
+    <col min="2819" max="2819" width="16.5" style="10" customWidth="1"/>
+    <col min="2820" max="2820" width="18.83203125" style="10" customWidth="1"/>
+    <col min="2821" max="2821" width="23.5" style="10" customWidth="1"/>
     <col min="2822" max="2822" width="13" style="10" customWidth="1"/>
     <col min="2823" max="3072" width="12" style="10"/>
-    <col min="3073" max="3073" width="13.6328125" style="10" customWidth="1"/>
+    <col min="3073" max="3073" width="13.6640625" style="10" customWidth="1"/>
     <col min="3074" max="3074" width="12" style="10"/>
-    <col min="3075" max="3075" width="16.453125" style="10" customWidth="1"/>
-    <col min="3076" max="3076" width="18.90625" style="10" customWidth="1"/>
-    <col min="3077" max="3077" width="23.54296875" style="10" customWidth="1"/>
+    <col min="3075" max="3075" width="16.5" style="10" customWidth="1"/>
+    <col min="3076" max="3076" width="18.83203125" style="10" customWidth="1"/>
+    <col min="3077" max="3077" width="23.5" style="10" customWidth="1"/>
     <col min="3078" max="3078" width="13" style="10" customWidth="1"/>
     <col min="3079" max="3328" width="12" style="10"/>
-    <col min="3329" max="3329" width="13.6328125" style="10" customWidth="1"/>
+    <col min="3329" max="3329" width="13.6640625" style="10" customWidth="1"/>
     <col min="3330" max="3330" width="12" style="10"/>
-    <col min="3331" max="3331" width="16.453125" style="10" customWidth="1"/>
-    <col min="3332" max="3332" width="18.90625" style="10" customWidth="1"/>
-    <col min="3333" max="3333" width="23.54296875" style="10" customWidth="1"/>
+    <col min="3331" max="3331" width="16.5" style="10" customWidth="1"/>
+    <col min="3332" max="3332" width="18.83203125" style="10" customWidth="1"/>
+    <col min="3333" max="3333" width="23.5" style="10" customWidth="1"/>
     <col min="3334" max="3334" width="13" style="10" customWidth="1"/>
     <col min="3335" max="3584" width="12" style="10"/>
-    <col min="3585" max="3585" width="13.6328125" style="10" customWidth="1"/>
+    <col min="3585" max="3585" width="13.6640625" style="10" customWidth="1"/>
     <col min="3586" max="3586" width="12" style="10"/>
-    <col min="3587" max="3587" width="16.453125" style="10" customWidth="1"/>
-    <col min="3588" max="3588" width="18.90625" style="10" customWidth="1"/>
-    <col min="3589" max="3589" width="23.54296875" style="10" customWidth="1"/>
+    <col min="3587" max="3587" width="16.5" style="10" customWidth="1"/>
+    <col min="3588" max="3588" width="18.83203125" style="10" customWidth="1"/>
+    <col min="3589" max="3589" width="23.5" style="10" customWidth="1"/>
     <col min="3590" max="3590" width="13" style="10" customWidth="1"/>
     <col min="3591" max="3840" width="12" style="10"/>
-    <col min="3841" max="3841" width="13.6328125" style="10" customWidth="1"/>
+    <col min="3841" max="3841" width="13.6640625" style="10" customWidth="1"/>
     <col min="3842" max="3842" width="12" style="10"/>
-    <col min="3843" max="3843" width="16.453125" style="10" customWidth="1"/>
-    <col min="3844" max="3844" width="18.90625" style="10" customWidth="1"/>
-    <col min="3845" max="3845" width="23.54296875" style="10" customWidth="1"/>
+    <col min="3843" max="3843" width="16.5" style="10" customWidth="1"/>
+    <col min="3844" max="3844" width="18.83203125" style="10" customWidth="1"/>
+    <col min="3845" max="3845" width="23.5" style="10" customWidth="1"/>
     <col min="3846" max="3846" width="13" style="10" customWidth="1"/>
     <col min="3847" max="4096" width="12" style="10"/>
-    <col min="4097" max="4097" width="13.6328125" style="10" customWidth="1"/>
+    <col min="4097" max="4097" width="13.6640625" style="10" customWidth="1"/>
     <col min="4098" max="4098" width="12" style="10"/>
-    <col min="4099" max="4099" width="16.453125" style="10" customWidth="1"/>
-    <col min="4100" max="4100" width="18.90625" style="10" customWidth="1"/>
-    <col min="4101" max="4101" width="23.54296875" style="10" customWidth="1"/>
+    <col min="4099" max="4099" width="16.5" style="10" customWidth="1"/>
+    <col min="4100" max="4100" width="18.83203125" style="10" customWidth="1"/>
+    <col min="4101" max="4101" width="23.5" style="10" customWidth="1"/>
     <col min="4102" max="4102" width="13" style="10" customWidth="1"/>
     <col min="4103" max="4352" width="12" style="10"/>
-    <col min="4353" max="4353" width="13.6328125" style="10" customWidth="1"/>
+    <col min="4353" max="4353" width="13.6640625" style="10" customWidth="1"/>
     <col min="4354" max="4354" width="12" style="10"/>
-    <col min="4355" max="4355" width="16.453125" style="10" customWidth="1"/>
-    <col min="4356" max="4356" width="18.90625" style="10" customWidth="1"/>
-    <col min="4357" max="4357" width="23.54296875" style="10" customWidth="1"/>
+    <col min="4355" max="4355" width="16.5" style="10" customWidth="1"/>
+    <col min="4356" max="4356" width="18.83203125" style="10" customWidth="1"/>
+    <col min="4357" max="4357" width="23.5" style="10" customWidth="1"/>
     <col min="4358" max="4358" width="13" style="10" customWidth="1"/>
     <col min="4359" max="4608" width="12" style="10"/>
-    <col min="4609" max="4609" width="13.6328125" style="10" customWidth="1"/>
+    <col min="4609" max="4609" width="13.6640625" style="10" customWidth="1"/>
     <col min="4610" max="4610" width="12" style="10"/>
-    <col min="4611" max="4611" width="16.453125" style="10" customWidth="1"/>
-    <col min="4612" max="4612" width="18.90625" style="10" customWidth="1"/>
-    <col min="4613" max="4613" width="23.54296875" style="10" customWidth="1"/>
+    <col min="4611" max="4611" width="16.5" style="10" customWidth="1"/>
+    <col min="4612" max="4612" width="18.83203125" style="10" customWidth="1"/>
+    <col min="4613" max="4613" width="23.5" style="10" customWidth="1"/>
     <col min="4614" max="4614" width="13" style="10" customWidth="1"/>
     <col min="4615" max="4864" width="12" style="10"/>
-    <col min="4865" max="4865" width="13.6328125" style="10" customWidth="1"/>
+    <col min="4865" max="4865" width="13.6640625" style="10" customWidth="1"/>
     <col min="4866" max="4866" width="12" style="10"/>
-    <col min="4867" max="4867" width="16.453125" style="10" customWidth="1"/>
-    <col min="4868" max="4868" width="18.90625" style="10" customWidth="1"/>
-    <col min="4869" max="4869" width="23.54296875" style="10" customWidth="1"/>
+    <col min="4867" max="4867" width="16.5" style="10" customWidth="1"/>
+    <col min="4868" max="4868" width="18.83203125" style="10" customWidth="1"/>
+    <col min="4869" max="4869" width="23.5" style="10" customWidth="1"/>
     <col min="4870" max="4870" width="13" style="10" customWidth="1"/>
     <col min="4871" max="5120" width="12" style="10"/>
-    <col min="5121" max="5121" width="13.6328125" style="10" customWidth="1"/>
+    <col min="5121" max="5121" width="13.6640625" style="10" customWidth="1"/>
     <col min="5122" max="5122" width="12" style="10"/>
-    <col min="5123" max="5123" width="16.453125" style="10" customWidth="1"/>
-    <col min="5124" max="5124" width="18.90625" style="10" customWidth="1"/>
-    <col min="5125" max="5125" width="23.54296875" style="10" customWidth="1"/>
+    <col min="5123" max="5123" width="16.5" style="10" customWidth="1"/>
+    <col min="5124" max="5124" width="18.83203125" style="10" customWidth="1"/>
+    <col min="5125" max="5125" width="23.5" style="10" customWidth="1"/>
     <col min="5126" max="5126" width="13" style="10" customWidth="1"/>
     <col min="5127" max="5376" width="12" style="10"/>
-    <col min="5377" max="5377" width="13.6328125" style="10" customWidth="1"/>
+    <col min="5377" max="5377" width="13.6640625" style="10" customWidth="1"/>
     <col min="5378" max="5378" width="12" style="10"/>
-    <col min="5379" max="5379" width="16.453125" style="10" customWidth="1"/>
-    <col min="5380" max="5380" width="18.90625" style="10" customWidth="1"/>
-    <col min="5381" max="5381" width="23.54296875" style="10" customWidth="1"/>
+    <col min="5379" max="5379" width="16.5" style="10" customWidth="1"/>
+    <col min="5380" max="5380" width="18.83203125" style="10" customWidth="1"/>
+    <col min="5381" max="5381" width="23.5" style="10" customWidth="1"/>
     <col min="5382" max="5382" width="13" style="10" customWidth="1"/>
     <col min="5383" max="5632" width="12" style="10"/>
-    <col min="5633" max="5633" width="13.6328125" style="10" customWidth="1"/>
+    <col min="5633" max="5633" width="13.6640625" style="10" customWidth="1"/>
     <col min="5634" max="5634" width="12" style="10"/>
-    <col min="5635" max="5635" width="16.453125" style="10" customWidth="1"/>
-    <col min="5636" max="5636" width="18.90625" style="10" customWidth="1"/>
-    <col min="5637" max="5637" width="23.54296875" style="10" customWidth="1"/>
+    <col min="5635" max="5635" width="16.5" style="10" customWidth="1"/>
+    <col min="5636" max="5636" width="18.83203125" style="10" customWidth="1"/>
+    <col min="5637" max="5637" width="23.5" style="10" customWidth="1"/>
     <col min="5638" max="5638" width="13" style="10" customWidth="1"/>
     <col min="5639" max="5888" width="12" style="10"/>
-    <col min="5889" max="5889" width="13.6328125" style="10" customWidth="1"/>
+    <col min="5889" max="5889" width="13.6640625" style="10" customWidth="1"/>
     <col min="5890" max="5890" width="12" style="10"/>
-    <col min="5891" max="5891" width="16.453125" style="10" customWidth="1"/>
-    <col min="5892" max="5892" width="18.90625" style="10" customWidth="1"/>
-    <col min="5893" max="5893" width="23.54296875" style="10" customWidth="1"/>
+    <col min="5891" max="5891" width="16.5" style="10" customWidth="1"/>
+    <col min="5892" max="5892" width="18.83203125" style="10" customWidth="1"/>
+    <col min="5893" max="5893" width="23.5" style="10" customWidth="1"/>
     <col min="5894" max="5894" width="13" style="10" customWidth="1"/>
     <col min="5895" max="6144" width="12" style="10"/>
-    <col min="6145" max="6145" width="13.6328125" style="10" customWidth="1"/>
+    <col min="6145" max="6145" width="13.6640625" style="10" customWidth="1"/>
     <col min="6146" max="6146" width="12" style="10"/>
-    <col min="6147" max="6147" width="16.453125" style="10" customWidth="1"/>
-    <col min="6148" max="6148" width="18.90625" style="10" customWidth="1"/>
-    <col min="6149" max="6149" width="23.54296875" style="10" customWidth="1"/>
+    <col min="6147" max="6147" width="16.5" style="10" customWidth="1"/>
+    <col min="6148" max="6148" width="18.83203125" style="10" customWidth="1"/>
+    <col min="6149" max="6149" width="23.5" style="10" customWidth="1"/>
     <col min="6150" max="6150" width="13" style="10" customWidth="1"/>
     <col min="6151" max="6400" width="12" style="10"/>
-    <col min="6401" max="6401" width="13.6328125" style="10" customWidth="1"/>
+    <col min="6401" max="6401" width="13.6640625" style="10" customWidth="1"/>
     <col min="6402" max="6402" width="12" style="10"/>
-    <col min="6403" max="6403" width="16.453125" style="10" customWidth="1"/>
-    <col min="6404" max="6404" width="18.90625" style="10" customWidth="1"/>
-    <col min="6405" max="6405" width="23.54296875" style="10" customWidth="1"/>
+    <col min="6403" max="6403" width="16.5" style="10" customWidth="1"/>
+    <col min="6404" max="6404" width="18.83203125" style="10" customWidth="1"/>
+    <col min="6405" max="6405" width="23.5" style="10" customWidth="1"/>
     <col min="6406" max="6406" width="13" style="10" customWidth="1"/>
     <col min="6407" max="6656" width="12" style="10"/>
-    <col min="6657" max="6657" width="13.6328125" style="10" customWidth="1"/>
+    <col min="6657" max="6657" width="13.6640625" style="10" customWidth="1"/>
     <col min="6658" max="6658" width="12" style="10"/>
-    <col min="6659" max="6659" width="16.453125" style="10" customWidth="1"/>
-    <col min="6660" max="6660" width="18.90625" style="10" customWidth="1"/>
-    <col min="6661" max="6661" width="23.54296875" style="10" customWidth="1"/>
+    <col min="6659" max="6659" width="16.5" style="10" customWidth="1"/>
+    <col min="6660" max="6660" width="18.83203125" style="10" customWidth="1"/>
+    <col min="6661" max="6661" width="23.5" style="10" customWidth="1"/>
     <col min="6662" max="6662" width="13" style="10" customWidth="1"/>
     <col min="6663" max="6912" width="12" style="10"/>
-    <col min="6913" max="6913" width="13.6328125" style="10" customWidth="1"/>
+    <col min="6913" max="6913" width="13.6640625" style="10" customWidth="1"/>
     <col min="6914" max="6914" width="12" style="10"/>
-    <col min="6915" max="6915" width="16.453125" style="10" customWidth="1"/>
-    <col min="6916" max="6916" width="18.90625" style="10" customWidth="1"/>
-    <col min="6917" max="6917" width="23.54296875" style="10" customWidth="1"/>
+    <col min="6915" max="6915" width="16.5" style="10" customWidth="1"/>
+    <col min="6916" max="6916" width="18.83203125" style="10" customWidth="1"/>
+    <col min="6917" max="6917" width="23.5" style="10" customWidth="1"/>
     <col min="6918" max="6918" width="13" style="10" customWidth="1"/>
     <col min="6919" max="7168" width="12" style="10"/>
-    <col min="7169" max="7169" width="13.6328125" style="10" customWidth="1"/>
+    <col min="7169" max="7169" width="13.6640625" style="10" customWidth="1"/>
     <col min="7170" max="7170" width="12" style="10"/>
-    <col min="7171" max="7171" width="16.453125" style="10" customWidth="1"/>
-    <col min="7172" max="7172" width="18.90625" style="10" customWidth="1"/>
-    <col min="7173" max="7173" width="23.54296875" style="10" customWidth="1"/>
+    <col min="7171" max="7171" width="16.5" style="10" customWidth="1"/>
+    <col min="7172" max="7172" width="18.83203125" style="10" customWidth="1"/>
+    <col min="7173" max="7173" width="23.5" style="10" customWidth="1"/>
     <col min="7174" max="7174" width="13" style="10" customWidth="1"/>
     <col min="7175" max="7424" width="12" style="10"/>
-    <col min="7425" max="7425" width="13.6328125" style="10" customWidth="1"/>
+    <col min="7425" max="7425" width="13.6640625" style="10" customWidth="1"/>
     <col min="7426" max="7426" width="12" style="10"/>
-    <col min="7427" max="7427" width="16.453125" style="10" customWidth="1"/>
-    <col min="7428" max="7428" width="18.90625" style="10" customWidth="1"/>
-    <col min="7429" max="7429" width="23.54296875" style="10" customWidth="1"/>
+    <col min="7427" max="7427" width="16.5" style="10" customWidth="1"/>
+    <col min="7428" max="7428" width="18.83203125" style="10" customWidth="1"/>
+    <col min="7429" max="7429" width="23.5" style="10" customWidth="1"/>
     <col min="7430" max="7430" width="13" style="10" customWidth="1"/>
     <col min="7431" max="7680" width="12" style="10"/>
-    <col min="7681" max="7681" width="13.6328125" style="10" customWidth="1"/>
+    <col min="7681" max="7681" width="13.6640625" style="10" customWidth="1"/>
     <col min="7682" max="7682" width="12" style="10"/>
-    <col min="7683" max="7683" width="16.453125" style="10" customWidth="1"/>
-    <col min="7684" max="7684" width="18.90625" style="10" customWidth="1"/>
-    <col min="7685" max="7685" width="23.54296875" style="10" customWidth="1"/>
+    <col min="7683" max="7683" width="16.5" style="10" customWidth="1"/>
+    <col min="7684" max="7684" width="18.83203125" style="10" customWidth="1"/>
+    <col min="7685" max="7685" width="23.5" style="10" customWidth="1"/>
     <col min="7686" max="7686" width="13" style="10" customWidth="1"/>
     <col min="7687" max="7936" width="12" style="10"/>
-    <col min="7937" max="7937" width="13.6328125" style="10" customWidth="1"/>
+    <col min="7937" max="7937" width="13.6640625" style="10" customWidth="1"/>
     <col min="7938" max="7938" width="12" style="10"/>
-    <col min="7939" max="7939" width="16.453125" style="10" customWidth="1"/>
-    <col min="7940" max="7940" width="18.90625" style="10" customWidth="1"/>
-    <col min="7941" max="7941" width="23.54296875" style="10" customWidth="1"/>
+    <col min="7939" max="7939" width="16.5" style="10" customWidth="1"/>
+    <col min="7940" max="7940" width="18.83203125" style="10" customWidth="1"/>
+    <col min="7941" max="7941" width="23.5" style="10" customWidth="1"/>
     <col min="7942" max="7942" width="13" style="10" customWidth="1"/>
     <col min="7943" max="8192" width="12" style="10"/>
-    <col min="8193" max="8193" width="13.6328125" style="10" customWidth="1"/>
+    <col min="8193" max="8193" width="13.6640625" style="10" customWidth="1"/>
     <col min="8194" max="8194" width="12" style="10"/>
-    <col min="8195" max="8195" width="16.453125" style="10" customWidth="1"/>
-    <col min="8196" max="8196" width="18.90625" style="10" customWidth="1"/>
-    <col min="8197" max="8197" width="23.54296875" style="10" customWidth="1"/>
+    <col min="8195" max="8195" width="16.5" style="10" customWidth="1"/>
+    <col min="8196" max="8196" width="18.83203125" style="10" customWidth="1"/>
+    <col min="8197" max="8197" width="23.5" style="10" customWidth="1"/>
     <col min="8198" max="8198" width="13" style="10" customWidth="1"/>
     <col min="8199" max="8448" width="12" style="10"/>
-    <col min="8449" max="8449" width="13.6328125" style="10" customWidth="1"/>
+    <col min="8449" max="8449" width="13.6640625" style="10" customWidth="1"/>
     <col min="8450" max="8450" width="12" style="10"/>
-    <col min="8451" max="8451" width="16.453125" style="10" customWidth="1"/>
-    <col min="8452" max="8452" width="18.90625" style="10" customWidth="1"/>
-    <col min="8453" max="8453" width="23.54296875" style="10" customWidth="1"/>
+    <col min="8451" max="8451" width="16.5" style="10" customWidth="1"/>
+    <col min="8452" max="8452" width="18.83203125" style="10" customWidth="1"/>
+    <col min="8453" max="8453" width="23.5" style="10" customWidth="1"/>
     <col min="8454" max="8454" width="13" style="10" customWidth="1"/>
     <col min="8455" max="8704" width="12" style="10"/>
-    <col min="8705" max="8705" width="13.6328125" style="10" customWidth="1"/>
+    <col min="8705" max="8705" width="13.6640625" style="10" customWidth="1"/>
     <col min="8706" max="8706" width="12" style="10"/>
-    <col min="8707" max="8707" width="16.453125" style="10" customWidth="1"/>
-    <col min="8708" max="8708" width="18.90625" style="10" customWidth="1"/>
-    <col min="8709" max="8709" width="23.54296875" style="10" customWidth="1"/>
+    <col min="8707" max="8707" width="16.5" style="10" customWidth="1"/>
+    <col min="8708" max="8708" width="18.83203125" style="10" customWidth="1"/>
+    <col min="8709" max="8709" width="23.5" style="10" customWidth="1"/>
     <col min="8710" max="8710" width="13" style="10" customWidth="1"/>
     <col min="8711" max="8960" width="12" style="10"/>
-    <col min="8961" max="8961" width="13.6328125" style="10" customWidth="1"/>
+    <col min="8961" max="8961" width="13.6640625" style="10" customWidth="1"/>
     <col min="8962" max="8962" width="12" style="10"/>
-    <col min="8963" max="8963" width="16.453125" style="10" customWidth="1"/>
-    <col min="8964" max="8964" width="18.90625" style="10" customWidth="1"/>
-    <col min="8965" max="8965" width="23.54296875" style="10" customWidth="1"/>
+    <col min="8963" max="8963" width="16.5" style="10" customWidth="1"/>
+    <col min="8964" max="8964" width="18.83203125" style="10" customWidth="1"/>
+    <col min="8965" max="8965" width="23.5" style="10" customWidth="1"/>
     <col min="8966" max="8966" width="13" style="10" customWidth="1"/>
     <col min="8967" max="9216" width="12" style="10"/>
-    <col min="9217" max="9217" width="13.6328125" style="10" customWidth="1"/>
+    <col min="9217" max="9217" width="13.6640625" style="10" customWidth="1"/>
     <col min="9218" max="9218" width="12" style="10"/>
-    <col min="9219" max="9219" width="16.453125" style="10" customWidth="1"/>
-    <col min="9220" max="9220" width="18.90625" style="10" customWidth="1"/>
-    <col min="9221" max="9221" width="23.54296875" style="10" customWidth="1"/>
+    <col min="9219" max="9219" width="16.5" style="10" customWidth="1"/>
+    <col min="9220" max="9220" width="18.83203125" style="10" customWidth="1"/>
+    <col min="9221" max="9221" width="23.5" style="10" customWidth="1"/>
     <col min="9222" max="9222" width="13" style="10" customWidth="1"/>
     <col min="9223" max="9472" width="12" style="10"/>
-    <col min="9473" max="9473" width="13.6328125" style="10" customWidth="1"/>
+    <col min="9473" max="9473" width="13.6640625" style="10" customWidth="1"/>
     <col min="9474" max="9474" width="12" style="10"/>
-    <col min="9475" max="9475" width="16.453125" style="10" customWidth="1"/>
-    <col min="9476" max="9476" width="18.90625" style="10" customWidth="1"/>
-    <col min="9477" max="9477" width="23.54296875" style="10" customWidth="1"/>
+    <col min="9475" max="9475" width="16.5" style="10" customWidth="1"/>
+    <col min="9476" max="9476" width="18.83203125" style="10" customWidth="1"/>
+    <col min="9477" max="9477" width="23.5" style="10" customWidth="1"/>
     <col min="9478" max="9478" width="13" style="10" customWidth="1"/>
     <col min="9479" max="9728" width="12" style="10"/>
-    <col min="9729" max="9729" width="13.6328125" style="10" customWidth="1"/>
+    <col min="9729" max="9729" width="13.6640625" style="10" customWidth="1"/>
     <col min="9730" max="9730" width="12" style="10"/>
-    <col min="9731" max="9731" width="16.453125" style="10" customWidth="1"/>
-    <col min="9732" max="9732" width="18.90625" style="10" customWidth="1"/>
-    <col min="9733" max="9733" width="23.54296875" style="10" customWidth="1"/>
+    <col min="9731" max="9731" width="16.5" style="10" customWidth="1"/>
+    <col min="9732" max="9732" width="18.83203125" style="10" customWidth="1"/>
+    <col min="9733" max="9733" width="23.5" style="10" customWidth="1"/>
     <col min="9734" max="9734" width="13" style="10" customWidth="1"/>
     <col min="9735" max="9984" width="12" style="10"/>
-    <col min="9985" max="9985" width="13.6328125" style="10" customWidth="1"/>
+    <col min="9985" max="9985" width="13.6640625" style="10" customWidth="1"/>
     <col min="9986" max="9986" width="12" style="10"/>
-    <col min="9987" max="9987" width="16.453125" style="10" customWidth="1"/>
-    <col min="9988" max="9988" width="18.90625" style="10" customWidth="1"/>
-    <col min="9989" max="9989" width="23.54296875" style="10" customWidth="1"/>
+    <col min="9987" max="9987" width="16.5" style="10" customWidth="1"/>
+    <col min="9988" max="9988" width="18.83203125" style="10" customWidth="1"/>
+    <col min="9989" max="9989" width="23.5" style="10" customWidth="1"/>
     <col min="9990" max="9990" width="13" style="10" customWidth="1"/>
     <col min="9991" max="10240" width="12" style="10"/>
-    <col min="10241" max="10241" width="13.6328125" style="10" customWidth="1"/>
+    <col min="10241" max="10241" width="13.6640625" style="10" customWidth="1"/>
     <col min="10242" max="10242" width="12" style="10"/>
-    <col min="10243" max="10243" width="16.453125" style="10" customWidth="1"/>
-    <col min="10244" max="10244" width="18.90625" style="10" customWidth="1"/>
-    <col min="10245" max="10245" width="23.54296875" style="10" customWidth="1"/>
+    <col min="10243" max="10243" width="16.5" style="10" customWidth="1"/>
+    <col min="10244" max="10244" width="18.83203125" style="10" customWidth="1"/>
+    <col min="10245" max="10245" width="23.5" style="10" customWidth="1"/>
     <col min="10246" max="10246" width="13" style="10" customWidth="1"/>
     <col min="10247" max="10496" width="12" style="10"/>
-    <col min="10497" max="10497" width="13.6328125" style="10" customWidth="1"/>
+    <col min="10497" max="10497" width="13.6640625" style="10" customWidth="1"/>
     <col min="10498" max="10498" width="12" style="10"/>
-    <col min="10499" max="10499" width="16.453125" style="10" customWidth="1"/>
-    <col min="10500" max="10500" width="18.90625" style="10" customWidth="1"/>
-    <col min="10501" max="10501" width="23.54296875" style="10" customWidth="1"/>
+    <col min="10499" max="10499" width="16.5" style="10" customWidth="1"/>
+    <col min="10500" max="10500" width="18.83203125" style="10" customWidth="1"/>
+    <col min="10501" max="10501" width="23.5" style="10" customWidth="1"/>
     <col min="10502" max="10502" width="13" style="10" customWidth="1"/>
     <col min="10503" max="10752" width="12" style="10"/>
-    <col min="10753" max="10753" width="13.6328125" style="10" customWidth="1"/>
+    <col min="10753" max="10753" width="13.6640625" style="10" customWidth="1"/>
     <col min="10754" max="10754" width="12" style="10"/>
-    <col min="10755" max="10755" width="16.453125" style="10" customWidth="1"/>
-    <col min="10756" max="10756" width="18.90625" style="10" customWidth="1"/>
-    <col min="10757" max="10757" width="23.54296875" style="10" customWidth="1"/>
+    <col min="10755" max="10755" width="16.5" style="10" customWidth="1"/>
+    <col min="10756" max="10756" width="18.83203125" style="10" customWidth="1"/>
+    <col min="10757" max="10757" width="23.5" style="10" customWidth="1"/>
     <col min="10758" max="10758" width="13" style="10" customWidth="1"/>
     <col min="10759" max="11008" width="12" style="10"/>
-    <col min="11009" max="11009" width="13.6328125" style="10" customWidth="1"/>
+    <col min="11009" max="11009" width="13.6640625" style="10" customWidth="1"/>
     <col min="11010" max="11010" width="12" style="10"/>
-    <col min="11011" max="11011" width="16.453125" style="10" customWidth="1"/>
-    <col min="11012" max="11012" width="18.90625" style="10" customWidth="1"/>
-    <col min="11013" max="11013" width="23.54296875" style="10" customWidth="1"/>
+    <col min="11011" max="11011" width="16.5" style="10" customWidth="1"/>
+    <col min="11012" max="11012" width="18.83203125" style="10" customWidth="1"/>
+    <col min="11013" max="11013" width="23.5" style="10" customWidth="1"/>
     <col min="11014" max="11014" width="13" style="10" customWidth="1"/>
     <col min="11015" max="11264" width="12" style="10"/>
-    <col min="11265" max="11265" width="13.6328125" style="10" customWidth="1"/>
+    <col min="11265" max="11265" width="13.6640625" style="10" customWidth="1"/>
     <col min="11266" max="11266" width="12" style="10"/>
-    <col min="11267" max="11267" width="16.453125" style="10" customWidth="1"/>
-    <col min="11268" max="11268" width="18.90625" style="10" customWidth="1"/>
-    <col min="11269" max="11269" width="23.54296875" style="10" customWidth="1"/>
+    <col min="11267" max="11267" width="16.5" style="10" customWidth="1"/>
+    <col min="11268" max="11268" width="18.83203125" style="10" customWidth="1"/>
+    <col min="11269" max="11269" width="23.5" style="10" customWidth="1"/>
     <col min="11270" max="11270" width="13" style="10" customWidth="1"/>
     <col min="11271" max="11520" width="12" style="10"/>
-    <col min="11521" max="11521" width="13.6328125" style="10" customWidth="1"/>
+    <col min="11521" max="11521" width="13.6640625" style="10" customWidth="1"/>
     <col min="11522" max="11522" width="12" style="10"/>
-    <col min="11523" max="11523" width="16.453125" style="10" customWidth="1"/>
-    <col min="11524" max="11524" width="18.90625" style="10" customWidth="1"/>
-    <col min="11525" max="11525" width="23.54296875" style="10" customWidth="1"/>
+    <col min="11523" max="11523" width="16.5" style="10" customWidth="1"/>
+    <col min="11524" max="11524" width="18.83203125" style="10" customWidth="1"/>
+    <col min="11525" max="11525" width="23.5" style="10" customWidth="1"/>
     <col min="11526" max="11526" width="13" style="10" customWidth="1"/>
     <col min="11527" max="11776" width="12" style="10"/>
-    <col min="11777" max="11777" width="13.6328125" style="10" customWidth="1"/>
+    <col min="11777" max="11777" width="13.6640625" style="10" customWidth="1"/>
     <col min="11778" max="11778" width="12" style="10"/>
-    <col min="11779" max="11779" width="16.453125" style="10" customWidth="1"/>
-    <col min="11780" max="11780" width="18.90625" style="10" customWidth="1"/>
-    <col min="11781" max="11781" width="23.54296875" style="10" customWidth="1"/>
+    <col min="11779" max="11779" width="16.5" style="10" customWidth="1"/>
+    <col min="11780" max="11780" width="18.83203125" style="10" customWidth="1"/>
+    <col min="11781" max="11781" width="23.5" style="10" customWidth="1"/>
     <col min="11782" max="11782" width="13" style="10" customWidth="1"/>
     <col min="11783" max="12032" width="12" style="10"/>
-    <col min="12033" max="12033" width="13.6328125" style="10" customWidth="1"/>
+    <col min="12033" max="12033" width="13.6640625" style="10" customWidth="1"/>
     <col min="12034" max="12034" width="12" style="10"/>
-    <col min="12035" max="12035" width="16.453125" style="10" customWidth="1"/>
-    <col min="12036" max="12036" width="18.90625" style="10" customWidth="1"/>
-    <col min="12037" max="12037" width="23.54296875" style="10" customWidth="1"/>
+    <col min="12035" max="12035" width="16.5" style="10" customWidth="1"/>
+    <col min="12036" max="12036" width="18.83203125" style="10" customWidth="1"/>
+    <col min="12037" max="12037" width="23.5" style="10" customWidth="1"/>
     <col min="12038" max="12038" width="13" style="10" customWidth="1"/>
     <col min="12039" max="12288" width="12" style="10"/>
-    <col min="12289" max="12289" width="13.6328125" style="10" customWidth="1"/>
+    <col min="12289" max="12289" width="13.6640625" style="10" customWidth="1"/>
     <col min="12290" max="12290" width="12" style="10"/>
-    <col min="12291" max="12291" width="16.453125" style="10" customWidth="1"/>
-    <col min="12292" max="12292" width="18.90625" style="10" customWidth="1"/>
-    <col min="12293" max="12293" width="23.54296875" style="10" customWidth="1"/>
+    <col min="12291" max="12291" width="16.5" style="10" customWidth="1"/>
+    <col min="12292" max="12292" width="18.83203125" style="10" customWidth="1"/>
+    <col min="12293" max="12293" width="23.5" style="10" customWidth="1"/>
     <col min="12294" max="12294" width="13" style="10" customWidth="1"/>
     <col min="12295" max="12544" width="12" style="10"/>
-    <col min="12545" max="12545" width="13.6328125" style="10" customWidth="1"/>
+    <col min="12545" max="12545" width="13.6640625" style="10" customWidth="1"/>
     <col min="12546" max="12546" width="12" style="10"/>
-    <col min="12547" max="12547" width="16.453125" style="10" customWidth="1"/>
-    <col min="12548" max="12548" width="18.90625" style="10" customWidth="1"/>
-    <col min="12549" max="12549" width="23.54296875" style="10" customWidth="1"/>
+    <col min="12547" max="12547" width="16.5" style="10" customWidth="1"/>
+    <col min="12548" max="12548" width="18.83203125" style="10" customWidth="1"/>
+    <col min="12549" max="12549" width="23.5" style="10" customWidth="1"/>
     <col min="12550" max="12550" width="13" style="10" customWidth="1"/>
     <col min="12551" max="12800" width="12" style="10"/>
-    <col min="12801" max="12801" width="13.6328125" style="10" customWidth="1"/>
+    <col min="12801" max="12801" width="13.6640625" style="10" customWidth="1"/>
     <col min="12802" max="12802" width="12" style="10"/>
-    <col min="12803" max="12803" width="16.453125" style="10" customWidth="1"/>
-    <col min="12804" max="12804" width="18.90625" style="10" customWidth="1"/>
-    <col min="12805" max="12805" width="23.54296875" style="10" customWidth="1"/>
+    <col min="12803" max="12803" width="16.5" style="10" customWidth="1"/>
+    <col min="12804" max="12804" width="18.83203125" style="10" customWidth="1"/>
+    <col min="12805" max="12805" width="23.5" style="10" customWidth="1"/>
     <col min="12806" max="12806" width="13" style="10" customWidth="1"/>
     <col min="12807" max="13056" width="12" style="10"/>
-    <col min="13057" max="13057" width="13.6328125" style="10" customWidth="1"/>
+    <col min="13057" max="13057" width="13.6640625" style="10" customWidth="1"/>
     <col min="13058" max="13058" width="12" style="10"/>
-    <col min="13059" max="13059" width="16.453125" style="10" customWidth="1"/>
-    <col min="13060" max="13060" width="18.90625" style="10" customWidth="1"/>
-    <col min="13061" max="13061" width="23.54296875" style="10" customWidth="1"/>
+    <col min="13059" max="13059" width="16.5" style="10" customWidth="1"/>
+    <col min="13060" max="13060" width="18.83203125" style="10" customWidth="1"/>
+    <col min="13061" max="13061" width="23.5" style="10" customWidth="1"/>
     <col min="13062" max="13062" width="13" style="10" customWidth="1"/>
     <col min="13063" max="13312" width="12" style="10"/>
-    <col min="13313" max="13313" width="13.6328125" style="10" customWidth="1"/>
+    <col min="13313" max="13313" width="13.6640625" style="10" customWidth="1"/>
     <col min="13314" max="13314" width="12" style="10"/>
-    <col min="13315" max="13315" width="16.453125" style="10" customWidth="1"/>
-    <col min="13316" max="13316" width="18.90625" style="10" customWidth="1"/>
-    <col min="13317" max="13317" width="23.54296875" style="10" customWidth="1"/>
+    <col min="13315" max="13315" width="16.5" style="10" customWidth="1"/>
+    <col min="13316" max="13316" width="18.83203125" style="10" customWidth="1"/>
+    <col min="13317" max="13317" width="23.5" style="10" customWidth="1"/>
     <col min="13318" max="13318" width="13" style="10" customWidth="1"/>
     <col min="13319" max="13568" width="12" style="10"/>
-    <col min="13569" max="13569" width="13.6328125" style="10" customWidth="1"/>
+    <col min="13569" max="13569" width="13.6640625" style="10" customWidth="1"/>
     <col min="13570" max="13570" width="12" style="10"/>
-    <col min="13571" max="13571" width="16.453125" style="10" customWidth="1"/>
-    <col min="13572" max="13572" width="18.90625" style="10" customWidth="1"/>
-    <col min="13573" max="13573" width="23.54296875" style="10" customWidth="1"/>
+    <col min="13571" max="13571" width="16.5" style="10" customWidth="1"/>
+    <col min="13572" max="13572" width="18.83203125" style="10" customWidth="1"/>
+    <col min="13573" max="13573" width="23.5" style="10" customWidth="1"/>
     <col min="13574" max="13574" width="13" style="10" customWidth="1"/>
     <col min="13575" max="13824" width="12" style="10"/>
-    <col min="13825" max="13825" width="13.6328125" style="10" customWidth="1"/>
+    <col min="13825" max="13825" width="13.6640625" style="10" customWidth="1"/>
     <col min="13826" max="13826" width="12" style="10"/>
-    <col min="13827" max="13827" width="16.453125" style="10" customWidth="1"/>
-    <col min="13828" max="13828" width="18.90625" style="10" customWidth="1"/>
-    <col min="13829" max="13829" width="23.54296875" style="10" customWidth="1"/>
+    <col min="13827" max="13827" width="16.5" style="10" customWidth="1"/>
+    <col min="13828" max="13828" width="18.83203125" style="10" customWidth="1"/>
+    <col min="13829" max="13829" width="23.5" style="10" customWidth="1"/>
     <col min="13830" max="13830" width="13" style="10" customWidth="1"/>
     <col min="13831" max="14080" width="12" style="10"/>
-    <col min="14081" max="14081" width="13.6328125" style="10" customWidth="1"/>
+    <col min="14081" max="14081" width="13.6640625" style="10" customWidth="1"/>
     <col min="14082" max="14082" width="12" style="10"/>
-    <col min="14083" max="14083" width="16.453125" style="10" customWidth="1"/>
-    <col min="14084" max="14084" width="18.90625" style="10" customWidth="1"/>
-    <col min="14085" max="14085" width="23.54296875" style="10" customWidth="1"/>
+    <col min="14083" max="14083" width="16.5" style="10" customWidth="1"/>
+    <col min="14084" max="14084" width="18.83203125" style="10" customWidth="1"/>
+    <col min="14085" max="14085" width="23.5" style="10" customWidth="1"/>
     <col min="14086" max="14086" width="13" style="10" customWidth="1"/>
     <col min="14087" max="14336" width="12" style="10"/>
-    <col min="14337" max="14337" width="13.6328125" style="10" customWidth="1"/>
+    <col min="14337" max="14337" width="13.6640625" style="10" customWidth="1"/>
     <col min="14338" max="14338" width="12" style="10"/>
-    <col min="14339" max="14339" width="16.453125" style="10" customWidth="1"/>
-    <col min="14340" max="14340" width="18.90625" style="10" customWidth="1"/>
-    <col min="14341" max="14341" width="23.54296875" style="10" customWidth="1"/>
+    <col min="14339" max="14339" width="16.5" style="10" customWidth="1"/>
+    <col min="14340" max="14340" width="18.83203125" style="10" customWidth="1"/>
+    <col min="14341" max="14341" width="23.5" style="10" customWidth="1"/>
     <col min="14342" max="14342" width="13" style="10" customWidth="1"/>
     <col min="14343" max="14592" width="12" style="10"/>
-    <col min="14593" max="14593" width="13.6328125" style="10" customWidth="1"/>
+    <col min="14593" max="14593" width="13.6640625" style="10" customWidth="1"/>
     <col min="14594" max="14594" width="12" style="10"/>
-    <col min="14595" max="14595" width="16.453125" style="10" customWidth="1"/>
-    <col min="14596" max="14596" width="18.90625" style="10" customWidth="1"/>
-    <col min="14597" max="14597" width="23.54296875" style="10" customWidth="1"/>
+    <col min="14595" max="14595" width="16.5" style="10" customWidth="1"/>
+    <col min="14596" max="14596" width="18.83203125" style="10" customWidth="1"/>
+    <col min="14597" max="14597" width="23.5" style="10" customWidth="1"/>
     <col min="14598" max="14598" width="13" style="10" customWidth="1"/>
     <col min="14599" max="14848" width="12" style="10"/>
-    <col min="14849" max="14849" width="13.6328125" style="10" customWidth="1"/>
+    <col min="14849" max="14849" width="13.6640625" style="10" customWidth="1"/>
     <col min="14850" max="14850" width="12" style="10"/>
-    <col min="14851" max="14851" width="16.453125" style="10" customWidth="1"/>
-    <col min="14852" max="14852" width="18.90625" style="10" customWidth="1"/>
-    <col min="14853" max="14853" width="23.54296875" style="10" customWidth="1"/>
+    <col min="14851" max="14851" width="16.5" style="10" customWidth="1"/>
+    <col min="14852" max="14852" width="18.83203125" style="10" customWidth="1"/>
+    <col min="14853" max="14853" width="23.5" style="10" customWidth="1"/>
     <col min="14854" max="14854" width="13" style="10" customWidth="1"/>
     <col min="14855" max="15104" width="12" style="10"/>
-    <col min="15105" max="15105" width="13.6328125" style="10" customWidth="1"/>
+    <col min="15105" max="15105" width="13.6640625" style="10" customWidth="1"/>
     <col min="15106" max="15106" width="12" style="10"/>
-    <col min="15107" max="15107" width="16.453125" style="10" customWidth="1"/>
-    <col min="15108" max="15108" width="18.90625" style="10" customWidth="1"/>
-    <col min="15109" max="15109" width="23.54296875" style="10" customWidth="1"/>
+    <col min="15107" max="15107" width="16.5" style="10" customWidth="1"/>
+    <col min="15108" max="15108" width="18.83203125" style="10" customWidth="1"/>
+    <col min="15109" max="15109" width="23.5" style="10" customWidth="1"/>
     <col min="15110" max="15110" width="13" style="10" customWidth="1"/>
     <col min="15111" max="15360" width="12" style="10"/>
-    <col min="15361" max="15361" width="13.6328125" style="10" customWidth="1"/>
+    <col min="15361" max="15361" width="13.6640625" style="10" customWidth="1"/>
     <col min="15362" max="15362" width="12" style="10"/>
-    <col min="15363" max="15363" width="16.453125" style="10" customWidth="1"/>
-    <col min="15364" max="15364" width="18.90625" style="10" customWidth="1"/>
-    <col min="15365" max="15365" width="23.54296875" style="10" customWidth="1"/>
+    <col min="15363" max="15363" width="16.5" style="10" customWidth="1"/>
+    <col min="15364" max="15364" width="18.83203125" style="10" customWidth="1"/>
+    <col min="15365" max="15365" width="23.5" style="10" customWidth="1"/>
     <col min="15366" max="15366" width="13" style="10" customWidth="1"/>
     <col min="15367" max="15616" width="12" style="10"/>
-    <col min="15617" max="15617" width="13.6328125" style="10" customWidth="1"/>
+    <col min="15617" max="15617" width="13.6640625" style="10" customWidth="1"/>
     <col min="15618" max="15618" width="12" style="10"/>
-    <col min="15619" max="15619" width="16.453125" style="10" customWidth="1"/>
-    <col min="15620" max="15620" width="18.90625" style="10" customWidth="1"/>
-    <col min="15621" max="15621" width="23.54296875" style="10" customWidth="1"/>
+    <col min="15619" max="15619" width="16.5" style="10" customWidth="1"/>
+    <col min="15620" max="15620" width="18.83203125" style="10" customWidth="1"/>
+    <col min="15621" max="15621" width="23.5" style="10" customWidth="1"/>
     <col min="15622" max="15622" width="13" style="10" customWidth="1"/>
     <col min="15623" max="15872" width="12" style="10"/>
-    <col min="15873" max="15873" width="13.6328125" style="10" customWidth="1"/>
+    <col min="15873" max="15873" width="13.6640625" style="10" customWidth="1"/>
     <col min="15874" max="15874" width="12" style="10"/>
-    <col min="15875" max="15875" width="16.453125" style="10" customWidth="1"/>
-    <col min="15876" max="15876" width="18.90625" style="10" customWidth="1"/>
-    <col min="15877" max="15877" width="23.54296875" style="10" customWidth="1"/>
+    <col min="15875" max="15875" width="16.5" style="10" customWidth="1"/>
+    <col min="15876" max="15876" width="18.83203125" style="10" customWidth="1"/>
+    <col min="15877" max="15877" width="23.5" style="10" customWidth="1"/>
     <col min="15878" max="15878" width="13" style="10" customWidth="1"/>
     <col min="15879" max="16128" width="12" style="10"/>
-    <col min="16129" max="16129" width="13.6328125" style="10" customWidth="1"/>
+    <col min="16129" max="16129" width="13.6640625" style="10" customWidth="1"/>
     <col min="16130" max="16130" width="12" style="10"/>
-    <col min="16131" max="16131" width="16.453125" style="10" customWidth="1"/>
-    <col min="16132" max="16132" width="18.90625" style="10" customWidth="1"/>
-    <col min="16133" max="16133" width="23.54296875" style="10" customWidth="1"/>
+    <col min="16131" max="16131" width="16.5" style="10" customWidth="1"/>
+    <col min="16132" max="16132" width="18.83203125" style="10" customWidth="1"/>
+    <col min="16133" max="16133" width="23.5" style="10" customWidth="1"/>
     <col min="16134" max="16134" width="13" style="10" customWidth="1"/>
     <col min="16135" max="16384" width="12" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +2222,7 @@
       <c r="AM1" s="10"/>
       <c r="AN1" s="10"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
@@ -1992,7 +2242,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
@@ -2008,8 +2258,11 @@
       <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F3" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -2025,8 +2278,11 @@
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F4" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -2042,8 +2298,11 @@
       <c r="E5" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F5" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2051,7 +2310,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>15</v>
@@ -2059,8 +2318,11 @@
       <c r="E6" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F6" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -2076,8 +2338,11 @@
       <c r="E7" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F7" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -2093,8 +2358,11 @@
       <c r="E8" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F8" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
@@ -2110,8 +2378,11 @@
       <c r="E9" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F9" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
@@ -2127,8 +2398,11 @@
       <c r="E10" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F10" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
@@ -2144,8 +2418,11 @@
       <c r="E11" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F11" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -2161,8 +2438,11 @@
       <c r="E12" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F12" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>7</v>
       </c>
@@ -2178,8 +2458,11 @@
       <c r="E13" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F13" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
@@ -2195,8 +2478,11 @@
       <c r="E14" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F14" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>7</v>
       </c>
@@ -2212,8 +2498,11 @@
       <c r="E15" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -2228,6 +2517,9 @@
       </c>
       <c r="E16" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="F16" s="4">
+        <v>38231</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -2264,7 +2556,7 @@
       <c r="AM16" s="10"/>
       <c r="AN16" s="10"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -2284,7 +2576,7 @@
         <v>38626</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -2300,9 +2592,11 @@
       <c r="E18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F18" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -2318,9 +2612,11 @@
       <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F19" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -2336,8 +2632,11 @@
       <c r="E20" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F20" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -2353,8 +2652,11 @@
       <c r="E21" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F21" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
@@ -2369,6 +2671,9 @@
       </c>
       <c r="E22" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="F22" s="11">
+        <v>38626</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -2405,7 +2710,7 @@
       <c r="AM22" s="10"/>
       <c r="AN22" s="10"/>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>39</v>
       </c>
@@ -2425,7 +2730,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>39</v>
       </c>
@@ -2441,9 +2746,11 @@
       <c r="E24" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F24" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>39</v>
       </c>
@@ -2459,8 +2766,11 @@
       <c r="E25" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -2475,6 +2785,9 @@
       </c>
       <c r="E26" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="F26" s="4">
+        <v>38353</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -2511,7 +2824,7 @@
       <c r="AM26" s="10"/>
       <c r="AN26" s="10"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -2531,7 +2844,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>45</v>
       </c>
@@ -2547,9 +2860,11 @@
       <c r="E28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F28" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
@@ -2565,8 +2880,11 @@
       <c r="E29" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F29" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
@@ -2582,8 +2900,11 @@
       <c r="E30" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F30" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>45</v>
       </c>
@@ -2599,8 +2920,11 @@
       <c r="E31" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F31" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -2616,8 +2940,11 @@
       <c r="E32" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F32" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -2633,8 +2960,11 @@
       <c r="E33" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F33" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>45</v>
       </c>
@@ -2650,8 +2980,11 @@
       <c r="E34" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F34" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -2667,8 +3000,11 @@
       <c r="E35" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F35" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
@@ -2684,8 +3020,11 @@
       <c r="E36" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F36" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>45</v>
       </c>
@@ -2700,6 +3039,9 @@
       </c>
       <c r="E37" s="18" t="s">
         <v>29</v>
+      </c>
+      <c r="F37" s="4">
+        <v>38353</v>
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -2736,7 +3078,7 @@
       <c r="AM37" s="10"/>
       <c r="AN37" s="10"/>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
@@ -2756,7 +3098,7 @@
         <v>38626</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>57</v>
       </c>
@@ -2772,8 +3114,11 @@
       <c r="E39" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F39" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
@@ -2789,8 +3134,11 @@
       <c r="E40" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F40" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>57</v>
       </c>
@@ -2806,8 +3154,11 @@
       <c r="E41" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F41" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -2823,8 +3174,11 @@
       <c r="E42" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F42" s="11">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="43" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>57</v>
       </c>
@@ -2840,7 +3194,9 @@
       <c r="E43" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="11">
+        <v>38626</v>
+      </c>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
@@ -2876,7 +3232,7 @@
       <c r="AM43" s="10"/>
       <c r="AN43" s="10"/>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>64</v>
       </c>
@@ -2896,7 +3252,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>64</v>
       </c>
@@ -2912,8 +3268,11 @@
       <c r="E45" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F45" s="19">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>64</v>
       </c>
@@ -2929,7 +3288,9 @@
       <c r="E46" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="19">
+        <v>38231</v>
+      </c>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
@@ -2965,7 +3326,7 @@
       <c r="AM46" s="10"/>
       <c r="AN46" s="10"/>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>68</v>
       </c>
@@ -2985,7 +3346,7 @@
         <v>38626</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>68</v>
       </c>
@@ -3001,8 +3362,11 @@
       <c r="E48" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F48" s="19">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>68</v>
       </c>
@@ -3018,8 +3382,11 @@
       <c r="E49" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F49" s="19">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>68</v>
       </c>
@@ -3034,6 +3401,9 @@
       </c>
       <c r="E50" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="F50" s="19">
+        <v>38626</v>
       </c>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
@@ -3070,7 +3440,7 @@
       <c r="AM50" s="10"/>
       <c r="AN50" s="10"/>
     </row>
-    <row r="51" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>73</v>
       </c>
@@ -3124,7 +3494,7 @@
       <c r="AM51" s="10"/>
       <c r="AN51" s="10"/>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>73</v>
       </c>
@@ -3140,9 +3510,11 @@
       <c r="E52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F52" s="4">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>73</v>
       </c>
@@ -3157,6 +3529,9 @@
       </c>
       <c r="E53" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="F53" s="4">
+        <v>38261</v>
       </c>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
@@ -3193,7 +3568,7 @@
       <c r="AM53" s="10"/>
       <c r="AN53" s="10"/>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>78</v>
       </c>
@@ -3213,7 +3588,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>78</v>
       </c>
@@ -3229,9 +3604,11 @@
       <c r="E55" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="4"/>
-    </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F55" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>78</v>
       </c>
@@ -3247,9 +3624,11 @@
       <c r="E56" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="4"/>
-    </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F56" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>78</v>
       </c>
@@ -3265,14 +3644,14 @@
       <c r="E57" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>83</v>
+      <c r="F57" s="4">
+        <v>38353</v>
       </c>
       <c r="J57" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>78</v>
       </c>
@@ -3288,9 +3667,11 @@
       <c r="E58" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F58" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>78</v>
       </c>
@@ -3306,9 +3687,11 @@
       <c r="E59" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F59" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="60" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>78</v>
       </c>
@@ -3324,7 +3707,9 @@
       <c r="E60" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F60" s="3"/>
+      <c r="F60" s="4">
+        <v>38353</v>
+      </c>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
@@ -3360,7 +3745,7 @@
       <c r="AM60" s="10"/>
       <c r="AN60" s="10"/>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>87</v>
       </c>
@@ -3380,7 +3765,7 @@
         <v>38626</v>
       </c>
     </row>
-    <row r="62" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>87</v>
       </c>
@@ -3396,7 +3781,9 @@
       <c r="E62" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="16"/>
+      <c r="F62" s="19">
+        <v>38626</v>
+      </c>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
@@ -3432,7 +3819,7 @@
       <c r="AM62" s="10"/>
       <c r="AN62" s="10"/>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>90</v>
       </c>
@@ -3452,7 +3839,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="64" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
         <v>90</v>
       </c>
@@ -3468,9 +3855,11 @@
       <c r="E64" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F64" s="4">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>90</v>
       </c>
@@ -3486,7 +3875,9 @@
       <c r="E65" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F65" s="16"/>
+      <c r="F65" s="4">
+        <v>38261</v>
+      </c>
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
@@ -3522,7 +3913,7 @@
       <c r="AM65" s="10"/>
       <c r="AN65" s="10"/>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
         <v>94</v>
       </c>
@@ -3542,7 +3933,7 @@
         <v>36861</v>
       </c>
     </row>
-    <row r="67" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>94</v>
       </c>
@@ -3558,9 +3949,11 @@
       <c r="E67" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F67" s="11"/>
-    </row>
-    <row r="68" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F67" s="11">
+        <v>36861</v>
+      </c>
+    </row>
+    <row r="68" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
         <v>94</v>
       </c>
@@ -3576,8 +3969,11 @@
       <c r="E68" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F68" s="11">
+        <v>36861</v>
+      </c>
+    </row>
+    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
         <v>94</v>
       </c>
@@ -3593,8 +3989,11 @@
       <c r="E69" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="70" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F69" s="11">
+        <v>36861</v>
+      </c>
+    </row>
+    <row r="70" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>94</v>
       </c>
@@ -3610,7 +4009,9 @@
       <c r="E70" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F70" s="1"/>
+      <c r="F70" s="11">
+        <v>36861</v>
+      </c>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
@@ -3646,7 +4047,7 @@
       <c r="AM70" s="10"/>
       <c r="AN70" s="10"/>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>102</v>
       </c>
@@ -3666,7 +4067,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="72" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>102</v>
       </c>
@@ -3682,7 +4083,9 @@
       <c r="E72" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F72" s="1"/>
+      <c r="F72" s="19">
+        <v>38261</v>
+      </c>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
       <c r="I72" s="10"/>
@@ -3718,7 +4121,7 @@
       <c r="AM72" s="10"/>
       <c r="AN72" s="10"/>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>105</v>
       </c>
@@ -3738,7 +4141,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>105</v>
       </c>
@@ -3754,11 +4157,14 @@
       <c r="E74" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="F74" s="19">
+        <v>38200</v>
+      </c>
       <c r="G74" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>105</v>
       </c>
@@ -3774,11 +4180,14 @@
       <c r="E75" s="10" t="s">
         <v>101</v>
       </c>
+      <c r="F75" s="19">
+        <v>38200</v>
+      </c>
       <c r="G75" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>105</v>
       </c>
@@ -3793,6 +4202,9 @@
       </c>
       <c r="E76" s="5" t="s">
         <v>112</v>
+      </c>
+      <c r="F76" s="19">
+        <v>38200</v>
       </c>
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
@@ -3829,7 +4241,7 @@
       <c r="AM76" s="10"/>
       <c r="AN76" s="10"/>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>113</v>
       </c>
@@ -3849,7 +4261,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>113</v>
       </c>
@@ -3865,9 +4277,11 @@
       <c r="E78" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F78" s="4"/>
-    </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F78" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>113</v>
       </c>
@@ -3883,9 +4297,11 @@
       <c r="E79" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F79" s="4"/>
-    </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F79" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>113</v>
       </c>
@@ -3901,9 +4317,11 @@
       <c r="E80" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F80" s="4"/>
-    </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F80" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>113</v>
       </c>
@@ -3919,8 +4337,11 @@
       <c r="E81" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F81" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>113</v>
       </c>
@@ -3936,8 +4357,11 @@
       <c r="E82" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="83" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F82" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="83" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>113</v>
       </c>
@@ -3953,8 +4377,11 @@
       <c r="E83" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="84" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F83" s="4">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="84" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>113</v>
       </c>
@@ -3969,6 +4396,9 @@
       </c>
       <c r="E84" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="F84" s="4">
+        <v>38353</v>
       </c>
       <c r="G84" s="10"/>
       <c r="H84" s="10"/>
@@ -4005,7 +4435,7 @@
       <c r="AM84" s="10"/>
       <c r="AN84" s="10"/>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
         <v>122</v>
       </c>
@@ -4025,7 +4455,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
         <v>122</v>
       </c>
@@ -4041,8 +4471,11 @@
       <c r="E86" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F86" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
         <v>122</v>
       </c>
@@ -4058,8 +4491,11 @@
       <c r="E87" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F87" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
         <v>122</v>
       </c>
@@ -4075,8 +4511,11 @@
       <c r="E88" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F88" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
         <v>122</v>
       </c>
@@ -4092,8 +4531,11 @@
       <c r="E89" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F89" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
         <v>122</v>
       </c>
@@ -4109,8 +4551,11 @@
       <c r="E90" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="91" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F90" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="91" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>122</v>
       </c>
@@ -4125,6 +4570,9 @@
       </c>
       <c r="E91" s="18" t="s">
         <v>29</v>
+      </c>
+      <c r="F91" s="4">
+        <v>38231</v>
       </c>
       <c r="G91" s="10"/>
       <c r="H91" s="10"/>
@@ -4161,7 +4609,7 @@
       <c r="AM91" s="10"/>
       <c r="AN91" s="10"/>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
         <v>130</v>
       </c>
@@ -4181,7 +4629,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="93" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
         <v>130</v>
       </c>
@@ -4197,9 +4645,11 @@
       <c r="E93" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F93" s="4"/>
-    </row>
-    <row r="94" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F93" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="94" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>130</v>
       </c>
@@ -4207,13 +4657,16 @@
         <v>16</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D94" s="17">
         <v>42401</v>
       </c>
       <c r="E94" s="18" t="s">
         <v>13</v>
+      </c>
+      <c r="F94" s="4">
+        <v>38231</v>
       </c>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
@@ -4250,7 +4703,7 @@
       <c r="AM94" s="10"/>
       <c r="AN94" s="10"/>
     </row>
-    <row r="95" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>133</v>
       </c>
@@ -4270,7 +4723,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="96" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>133</v>
       </c>
@@ -4286,7 +4739,9 @@
       <c r="E96" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F96" s="16"/>
+      <c r="F96" s="20">
+        <v>38261</v>
+      </c>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
       <c r="I96" s="10"/>
@@ -4322,7 +4777,7 @@
       <c r="AM96" s="10"/>
       <c r="AN96" s="10"/>
     </row>
-    <row r="97" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>136</v>
       </c>
@@ -4342,7 +4797,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="98" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>136</v>
       </c>
@@ -4358,7 +4813,9 @@
       <c r="E98" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F98" s="3"/>
+      <c r="F98" s="20">
+        <v>38261</v>
+      </c>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
       <c r="I98" s="10"/>
@@ -4394,7 +4851,7 @@
       <c r="AM98" s="10"/>
       <c r="AN98" s="10"/>
     </row>
-    <row r="99" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>139</v>
       </c>
@@ -4414,7 +4871,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="100" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>139</v>
       </c>
@@ -4430,9 +4887,11 @@
       <c r="E100" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F100" s="20"/>
-    </row>
-    <row r="101" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F100" s="24">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="101" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>142</v>
       </c>
@@ -4448,7 +4907,9 @@
       <c r="E101" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F101" s="1"/>
+      <c r="F101" s="24">
+        <v>38353</v>
+      </c>
       <c r="G101" s="10"/>
       <c r="H101" s="10"/>
       <c r="I101" s="10"/>
@@ -4484,7 +4945,7 @@
       <c r="AM101" s="10"/>
       <c r="AN101" s="10"/>
     </row>
-    <row r="102" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>144</v>
       </c>
@@ -4504,7 +4965,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="103" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -4520,9 +4981,11 @@
       <c r="E103" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F103" s="20"/>
-    </row>
-    <row r="104" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F103" s="24">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="104" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>144</v>
       </c>
@@ -4538,9 +5001,11 @@
       <c r="E104" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F104" s="20"/>
-    </row>
-    <row r="105" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F104" s="24">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="105" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>144</v>
       </c>
@@ -4556,7 +5021,9 @@
       <c r="E105" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F105" s="16"/>
+      <c r="F105" s="24">
+        <v>38353</v>
+      </c>
       <c r="G105" s="10"/>
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
@@ -4592,7 +5059,7 @@
       <c r="AM105" s="10"/>
       <c r="AN105" s="10"/>
     </row>
-    <row r="106" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
         <v>142</v>
       </c>
@@ -4612,7 +5079,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="107" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
         <v>142</v>
       </c>
@@ -4628,8 +5095,11 @@
       <c r="E107" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="108" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F107" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>142</v>
       </c>
@@ -4645,9 +5115,11 @@
       <c r="E108" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F108" s="1"/>
-    </row>
-    <row r="109" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F108" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="109" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>142</v>
       </c>
@@ -4663,9 +5135,11 @@
       <c r="E109" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F109" s="5"/>
-    </row>
-    <row r="110" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F109" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="110" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>153</v>
       </c>
@@ -4685,7 +5159,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="111" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>153</v>
       </c>
@@ -4701,8 +5175,11 @@
       <c r="E111" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F111" s="25">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="112" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>153</v>
       </c>
@@ -4718,8 +5195,11 @@
       <c r="E112" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="113" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F112" s="25">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="113" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>153</v>
       </c>
@@ -4735,8 +5215,11 @@
       <c r="E113" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="114" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F113" s="25">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="114" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>153</v>
       </c>
@@ -4751,6 +5234,9 @@
       </c>
       <c r="E114" s="18" t="s">
         <v>29</v>
+      </c>
+      <c r="F114" s="25">
+        <v>38353</v>
       </c>
       <c r="G114" s="10"/>
       <c r="H114" s="10"/>
@@ -4787,7 +5273,7 @@
       <c r="AM114" s="10"/>
       <c r="AN114" s="10"/>
     </row>
-    <row r="115" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
         <v>159</v>
       </c>
@@ -4807,7 +5293,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="116" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
         <v>159</v>
       </c>
@@ -4823,9 +5309,11 @@
       <c r="E116" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F116" s="20"/>
-    </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F116" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="117" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
         <v>159</v>
       </c>
@@ -4841,8 +5329,11 @@
       <c r="E117" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="118" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F117" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="118" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
         <v>159</v>
       </c>
@@ -4858,8 +5349,11 @@
       <c r="E118" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="119" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F118" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="119" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>159</v>
       </c>
@@ -4875,7 +5369,9 @@
       <c r="E119" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F119" s="1"/>
+      <c r="F119" s="20">
+        <v>38261</v>
+      </c>
       <c r="G119" s="10"/>
       <c r="H119" s="10"/>
       <c r="I119" s="10"/>
@@ -4911,7 +5407,7 @@
       <c r="AM119" s="10"/>
       <c r="AN119" s="10"/>
     </row>
-    <row r="120" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
         <v>159</v>
       </c>
@@ -4927,8 +5423,11 @@
       <c r="E120" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="121" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F120" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="121" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
         <v>159</v>
       </c>
@@ -4944,8 +5443,11 @@
       <c r="E121" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="122" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F121" s="20">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>159</v>
       </c>
@@ -4961,7 +5463,9 @@
       <c r="E122" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F122" s="1"/>
+      <c r="F122" s="20">
+        <v>38261</v>
+      </c>
       <c r="G122" s="10"/>
       <c r="H122" s="10"/>
       <c r="I122" s="10"/>
@@ -4997,7 +5501,7 @@
       <c r="AM122" s="10"/>
       <c r="AN122" s="10"/>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>168</v>
       </c>
@@ -5017,7 +5521,7 @@
         <v>38626</v>
       </c>
     </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>168</v>
       </c>
@@ -5033,9 +5537,11 @@
       <c r="E124" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F124" s="4"/>
-    </row>
-    <row r="125" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F124" s="19">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="125" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>168</v>
       </c>
@@ -5051,9 +5557,11 @@
       <c r="E125" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F125" s="4"/>
-    </row>
-    <row r="126" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F125" s="19">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>168</v>
       </c>
@@ -5069,8 +5577,11 @@
       <c r="E126" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="127" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F126" s="19">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="127" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>168</v>
       </c>
@@ -5085,6 +5596,9 @@
       </c>
       <c r="E127" s="18" t="s">
         <v>22</v>
+      </c>
+      <c r="F127" s="19">
+        <v>38626</v>
       </c>
       <c r="G127" s="10"/>
       <c r="H127" s="10"/>
@@ -5121,7 +5635,7 @@
       <c r="AM127" s="10"/>
       <c r="AN127" s="10"/>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
         <v>174</v>
       </c>
@@ -5141,7 +5655,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
         <v>174</v>
       </c>
@@ -5157,8 +5671,11 @@
       <c r="E129" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="130" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F129" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="130" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
         <v>174</v>
       </c>
@@ -5174,8 +5691,11 @@
       <c r="E130" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F130" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
         <v>130</v>
       </c>
@@ -5191,8 +5711,11 @@
       <c r="E131" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="132" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F131" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="132" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
         <v>174</v>
       </c>
@@ -5208,8 +5731,11 @@
       <c r="E132" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="133" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F132" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="133" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
         <v>174</v>
       </c>
@@ -5225,9 +5751,11 @@
       <c r="E133" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F133" s="3"/>
-    </row>
-    <row r="134" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F133" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>174</v>
       </c>
@@ -5243,9 +5771,11 @@
       <c r="E134" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F134" s="3"/>
-    </row>
-    <row r="135" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F134" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
         <v>174</v>
       </c>
@@ -5261,8 +5791,11 @@
       <c r="E135" s="10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="136" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F135" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="136" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>174</v>
       </c>
@@ -5278,7 +5811,9 @@
       <c r="E136" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F136" s="1"/>
+      <c r="F136" s="4">
+        <v>38231</v>
+      </c>
       <c r="G136" s="1"/>
       <c r="H136" s="10"/>
       <c r="I136" s="10"/>
@@ -5314,7 +5849,7 @@
       <c r="AM136" s="10"/>
       <c r="AN136" s="10"/>
     </row>
-    <row r="137" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
         <v>184</v>
       </c>
@@ -5334,7 +5869,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="138" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
         <v>184</v>
       </c>
@@ -5350,9 +5885,11 @@
       <c r="E138" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F138" s="4"/>
-    </row>
-    <row r="139" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F138" s="19">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
         <v>184</v>
       </c>
@@ -5368,9 +5905,11 @@
       <c r="E139" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F139" s="4"/>
-    </row>
-    <row r="140" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F139" s="19">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
         <v>184</v>
       </c>
@@ -5386,9 +5925,11 @@
       <c r="E140" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F140" s="3"/>
-    </row>
-    <row r="141" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F140" s="19">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="141" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="10" t="s">
         <v>184</v>
       </c>
@@ -5404,9 +5945,11 @@
       <c r="E141" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F141" s="3"/>
-    </row>
-    <row r="142" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F141" s="19">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="142" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>184</v>
       </c>
@@ -5421,6 +5964,9 @@
       </c>
       <c r="E142" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="F142" s="19">
+        <v>38231</v>
       </c>
       <c r="G142" s="10"/>
       <c r="H142" s="10"/>
@@ -5457,7 +6003,7 @@
       <c r="AM142" s="10"/>
       <c r="AN142" s="10"/>
     </row>
-    <row r="143" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A143" s="10" t="s">
         <v>192</v>
       </c>
@@ -5477,7 +6023,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="144" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A144" s="10" t="s">
         <v>192</v>
       </c>
@@ -5493,9 +6039,11 @@
       <c r="E144" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F144" s="4"/>
-    </row>
-    <row r="145" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F144" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="145" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A145" s="10" t="s">
         <v>192</v>
       </c>
@@ -5511,9 +6059,11 @@
       <c r="E145" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F145" s="4"/>
-    </row>
-    <row r="146" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F145" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="146" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A146" s="10" t="s">
         <v>192</v>
       </c>
@@ -5529,8 +6079,11 @@
       <c r="E146" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="147" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F146" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="147" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="10" t="s">
         <v>192</v>
       </c>
@@ -5546,8 +6099,11 @@
       <c r="E147" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="148" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F147" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="148" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
         <v>192</v>
       </c>
@@ -5563,8 +6119,11 @@
       <c r="E148" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="149" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F148" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="149" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>192</v>
       </c>
@@ -5579,6 +6138,9 @@
       </c>
       <c r="E149" s="18" t="s">
         <v>29</v>
+      </c>
+      <c r="F149" s="4">
+        <v>38231</v>
       </c>
       <c r="G149" s="10"/>
       <c r="H149" s="10"/>
@@ -5615,7 +6177,7 @@
       <c r="AM149" s="10"/>
       <c r="AN149" s="10"/>
     </row>
-    <row r="150" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>200</v>
       </c>
@@ -5635,7 +6197,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="151" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>200</v>
       </c>
@@ -5651,8 +6213,11 @@
       <c r="E151" s="23" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="152" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F151" s="25">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="152" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>200</v>
       </c>
@@ -5668,8 +6233,11 @@
       <c r="E152" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="153" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F152" s="25">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="153" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>200</v>
       </c>
@@ -5685,8 +6253,11 @@
       <c r="E153" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="154" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F153" s="25">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="154" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>200</v>
       </c>
@@ -5702,8 +6273,11 @@
       <c r="E154" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="155" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F154" s="25">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="155" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>200</v>
       </c>
@@ -5718,6 +6292,9 @@
       </c>
       <c r="E155" s="18" t="s">
         <v>13</v>
+      </c>
+      <c r="F155" s="25">
+        <v>38261</v>
       </c>
       <c r="G155" s="10"/>
       <c r="H155" s="10"/>
@@ -5754,7 +6331,7 @@
       <c r="AM155" s="10"/>
       <c r="AN155" s="10"/>
     </row>
-    <row r="156" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>207</v>
       </c>
@@ -5774,7 +6351,7 @@
         <v>38261</v>
       </c>
     </row>
-    <row r="157" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
         <v>207</v>
       </c>
@@ -5789,6 +6366,9 @@
       </c>
       <c r="E157" s="18" t="s">
         <v>29</v>
+      </c>
+      <c r="F157" s="25">
+        <v>38261</v>
       </c>
       <c r="G157" s="10"/>
       <c r="H157" s="10"/>
@@ -5825,7 +6405,7 @@
       <c r="AM157" s="10"/>
       <c r="AN157" s="10"/>
     </row>
-    <row r="158" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A158" s="10" t="s">
         <v>210</v>
       </c>
@@ -5845,7 +6425,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="159" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="10" t="s">
         <v>210</v>
       </c>
@@ -5861,9 +6441,11 @@
       <c r="E159" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F159" s="4"/>
-    </row>
-    <row r="160" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F159" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="160" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A160" s="10" t="s">
         <v>210</v>
       </c>
@@ -5879,8 +6461,11 @@
       <c r="E160" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="161" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F160" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="161" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="10" t="s">
         <v>210</v>
       </c>
@@ -5896,8 +6481,11 @@
       <c r="E161" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="162" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F161" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="162" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A162" s="10" t="s">
         <v>210</v>
       </c>
@@ -5913,8 +6501,11 @@
       <c r="E162" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="163" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F162" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="163" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A163" s="10" t="s">
         <v>210</v>
       </c>
@@ -5930,8 +6521,11 @@
       <c r="E163" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="164" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F163" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="164" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A164" s="10" t="s">
         <v>210</v>
       </c>
@@ -5947,8 +6541,11 @@
       <c r="E164" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="165" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F164" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="165" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>210</v>
       </c>
@@ -5963,6 +6560,9 @@
       </c>
       <c r="E165" s="18" t="s">
         <v>29</v>
+      </c>
+      <c r="F165" s="4">
+        <v>38231</v>
       </c>
       <c r="G165" s="10"/>
       <c r="H165" s="10"/>
@@ -5999,7 +6599,7 @@
       <c r="AM165" s="10"/>
       <c r="AN165" s="10"/>
     </row>
-    <row r="166" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A166" s="10" t="s">
         <v>219</v>
       </c>
@@ -6019,7 +6619,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="167" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A167" s="10" t="s">
         <v>219</v>
       </c>
@@ -6035,8 +6635,11 @@
       <c r="E167" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="168" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F167" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="168" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A168" s="10" t="s">
         <v>219</v>
       </c>
@@ -6052,8 +6655,11 @@
       <c r="E168" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="169" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F168" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="169" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A169" s="10" t="s">
         <v>219</v>
       </c>
@@ -6069,8 +6675,11 @@
       <c r="E169" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="170" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F169" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="170" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="10" t="s">
         <v>219</v>
       </c>
@@ -6086,8 +6695,11 @@
       <c r="E170" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="171" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F170" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="171" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A171" s="10" t="s">
         <v>219</v>
       </c>
@@ -6103,8 +6715,11 @@
       <c r="E171" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="172" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F171" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="172" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
         <v>219</v>
       </c>
@@ -6119,6 +6734,9 @@
       </c>
       <c r="E172" s="18" t="s">
         <v>29</v>
+      </c>
+      <c r="F172" s="4">
+        <v>38231</v>
       </c>
       <c r="G172" s="10"/>
       <c r="H172" s="10"/>
@@ -6155,7 +6773,7 @@
       <c r="AM172" s="10"/>
       <c r="AN172" s="10"/>
     </row>
-    <row r="173" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>227</v>
       </c>
@@ -6175,7 +6793,7 @@
         <v>38231</v>
       </c>
     </row>
-    <row r="174" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>227</v>
       </c>
@@ -6191,9 +6809,11 @@
       <c r="E174" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F174" s="4"/>
-    </row>
-    <row r="175" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F174" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="175" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>227</v>
       </c>
@@ -6209,8 +6829,11 @@
       <c r="E175" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="176" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F175" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="176" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>227</v>
       </c>
@@ -6226,8 +6849,11 @@
       <c r="E176" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="177" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F176" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="177" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>227</v>
       </c>
@@ -6243,9 +6869,11 @@
       <c r="E177" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F177" s="3"/>
-    </row>
-    <row r="178" spans="1:40" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F177" s="4">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="178" spans="1:40" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="5" t="s">
         <v>227</v>
       </c>
@@ -6261,7 +6889,9 @@
       <c r="E178" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F178" s="16"/>
+      <c r="F178" s="4">
+        <v>38231</v>
+      </c>
       <c r="G178" s="10"/>
       <c r="H178" s="10"/>
       <c r="I178" s="10"/>
@@ -6297,7 +6927,7 @@
       <c r="AM178" s="10"/>
       <c r="AN178" s="10"/>
     </row>
-    <row r="179" spans="1:40" ht="17" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:40" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="10" t="s">
         <v>234</v>
       </c>
@@ -6317,7 +6947,7 @@
         <v>36617</v>
       </c>
     </row>
-    <row r="180" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="10" t="s">
         <v>234</v>
       </c>
@@ -6333,8 +6963,11 @@
       <c r="E180" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="181" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F180" s="11">
+        <v>36617</v>
+      </c>
+    </row>
+    <row r="181" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A181" s="10" t="s">
         <v>234</v>
       </c>
@@ -6350,8 +6983,11 @@
       <c r="E181" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="182" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F181" s="11">
+        <v>36617</v>
+      </c>
+    </row>
+    <row r="182" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="10" t="s">
         <v>234</v>
       </c>
@@ -6367,9 +7003,11 @@
       <c r="E182" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F182" s="3"/>
-    </row>
-    <row r="183" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F182" s="11">
+        <v>36617</v>
+      </c>
+    </row>
+    <row r="183" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A183" s="10" t="s">
         <v>234</v>
       </c>
@@ -6385,9 +7023,11 @@
       <c r="E183" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F183" s="3"/>
-    </row>
-    <row r="184" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F183" s="11">
+        <v>36617</v>
+      </c>
+    </row>
+    <row r="184" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="10" t="s">
         <v>234</v>
       </c>
@@ -6403,9 +7043,11 @@
       <c r="E184" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F184" s="3"/>
-    </row>
-    <row r="185" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F184" s="11">
+        <v>36617</v>
+      </c>
+    </row>
+    <row r="185" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" s="5" t="s">
         <v>234</v>
       </c>
@@ -6420,6 +7062,9 @@
       </c>
       <c r="E185" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="F185" s="11">
+        <v>36617</v>
       </c>
       <c r="G185" s="10"/>
       <c r="H185" s="10"/>
@@ -6456,7 +7101,7 @@
       <c r="AM185" s="10"/>
       <c r="AN185" s="10"/>
     </row>
-    <row r="186" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>244</v>
       </c>
@@ -6476,7 +7121,7 @@
         <v>36831</v>
       </c>
     </row>
-    <row r="187" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>244</v>
       </c>
@@ -6492,8 +7137,11 @@
       <c r="E187" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="188" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F187" s="11">
+        <v>36831</v>
+      </c>
+    </row>
+    <row r="188" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>244</v>
       </c>
@@ -6509,8 +7157,11 @@
       <c r="E188" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="189" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F188" s="11">
+        <v>36831</v>
+      </c>
+    </row>
+    <row r="189" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
         <v>244</v>
       </c>
@@ -6525,6 +7176,9 @@
       </c>
       <c r="E189" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="F189" s="11">
+        <v>36831</v>
       </c>
       <c r="G189" s="10"/>
       <c r="H189" s="10"/>
@@ -6561,7 +7215,7 @@
       <c r="AM189" s="10"/>
       <c r="AN189" s="10"/>
     </row>
-    <row r="190" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>250</v>
       </c>
@@ -6581,7 +7235,7 @@
         <v>37622</v>
       </c>
     </row>
-    <row r="191" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>250</v>
       </c>
@@ -6597,8 +7251,11 @@
       <c r="E191" s="10" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="192" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F191" s="11">
+        <v>37622</v>
+      </c>
+    </row>
+    <row r="192" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
         <v>250</v>
       </c>
@@ -6613,6 +7270,9 @@
       </c>
       <c r="E192" s="5" t="s">
         <v>253</v>
+      </c>
+      <c r="F192" s="11">
+        <v>37622</v>
       </c>
       <c r="G192" s="10"/>
       <c r="H192" s="10"/>
@@ -6649,7 +7309,7 @@
       <c r="AM192" s="10"/>
       <c r="AN192" s="10"/>
     </row>
-    <row r="193" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A193" s="10" t="s">
         <v>255</v>
       </c>
@@ -6669,7 +7329,7 @@
         <v>37257</v>
       </c>
     </row>
-    <row r="194" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A194" s="10" t="s">
         <v>255</v>
       </c>
@@ -6685,8 +7345,11 @@
       <c r="E194" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="195" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F194" s="11">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="195" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A195" s="10" t="s">
         <v>255</v>
       </c>
@@ -6702,8 +7365,11 @@
       <c r="E195" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="196" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F195" s="11">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="196" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A196" s="10" t="s">
         <v>255</v>
       </c>
@@ -6719,8 +7385,11 @@
       <c r="E196" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="197" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F196" s="11">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="197" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A197" s="10" t="s">
         <v>255</v>
       </c>
@@ -6736,8 +7405,11 @@
       <c r="E197" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="198" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F197" s="11">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="198" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A198" s="10" t="s">
         <v>255</v>
       </c>
@@ -6753,8 +7425,11 @@
       <c r="E198" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="199" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F198" s="11">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="199" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A199" s="10" t="s">
         <v>255</v>
       </c>
@@ -6770,8 +7445,11 @@
       <c r="E199" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="200" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F199" s="11">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="200" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
         <v>255</v>
       </c>
@@ -6786,6 +7464,9 @@
       </c>
       <c r="E200" s="5" t="s">
         <v>253</v>
+      </c>
+      <c r="F200" s="11">
+        <v>37257</v>
       </c>
       <c r="G200" s="10"/>
       <c r="H200" s="10"/>
@@ -6822,7 +7503,7 @@
       <c r="AM200" s="10"/>
       <c r="AN200" s="10"/>
     </row>
-    <row r="201" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:40" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>270</v>
       </c>
@@ -6842,7 +7523,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="202" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="5" t="s">
         <v>270</v>
       </c>
@@ -6857,6 +7538,9 @@
       </c>
       <c r="E202" s="5" t="s">
         <v>273</v>
+      </c>
+      <c r="F202" s="19">
+        <v>38200</v>
       </c>
       <c r="G202" s="10"/>
       <c r="H202" s="10"/>
@@ -6893,7 +7577,7 @@
       <c r="AM202" s="10"/>
       <c r="AN202" s="10"/>
     </row>
-    <row r="203" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>274</v>
       </c>
@@ -6909,11 +7593,8 @@
       <c r="E203" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="F203" s="10">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="204" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="204" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
         <v>274</v>
       </c>
@@ -6929,6 +7610,7 @@
       <c r="E204" s="5" t="s">
         <v>253</v>
       </c>
+      <c r="F204" s="10"/>
       <c r="G204" s="10"/>
       <c r="H204" s="10"/>
       <c r="I204" s="10"/>
@@ -6964,7 +7646,7 @@
       <c r="AM204" s="10"/>
       <c r="AN204" s="10"/>
     </row>
-    <row r="205" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A205" s="10" t="s">
         <v>277</v>
       </c>
@@ -6984,7 +7666,7 @@
         <v>36831</v>
       </c>
     </row>
-    <row r="206" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="5" t="s">
         <v>277</v>
       </c>
@@ -6999,6 +7681,9 @@
       </c>
       <c r="E206" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="F206" s="11">
+        <v>36831</v>
       </c>
       <c r="G206" s="10"/>
       <c r="H206" s="10"/>
@@ -7035,7 +7720,7 @@
       <c r="AM206" s="10"/>
       <c r="AN206" s="10"/>
     </row>
-    <row r="207" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>280</v>
       </c>
@@ -7055,7 +7740,7 @@
         <v>40940</v>
       </c>
     </row>
-    <row r="208" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="5" t="s">
         <v>280</v>
       </c>
@@ -7070,6 +7755,9 @@
       </c>
       <c r="E208" s="5" t="s">
         <v>253</v>
+      </c>
+      <c r="F208" s="11">
+        <v>40940</v>
       </c>
       <c r="G208" s="10"/>
       <c r="H208" s="10"/>
@@ -7106,7 +7794,7 @@
       <c r="AM208" s="10"/>
       <c r="AN208" s="10"/>
     </row>
-    <row r="209" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A209" s="10" t="s">
         <v>283</v>
       </c>
@@ -7126,7 +7814,7 @@
         <v>39661</v>
       </c>
     </row>
-    <row r="210" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
         <v>283</v>
       </c>
@@ -7141,6 +7829,9 @@
       </c>
       <c r="E210" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="F210" s="11">
+        <v>39661</v>
       </c>
       <c r="G210" s="10"/>
       <c r="H210" s="10"/>
@@ -7177,7 +7868,7 @@
       <c r="AM210" s="10"/>
       <c r="AN210" s="10"/>
     </row>
-    <row r="211" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>286</v>
       </c>
@@ -7197,7 +7888,7 @@
         <v>40057</v>
       </c>
     </row>
-    <row r="212" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212" s="5" t="s">
         <v>286</v>
       </c>
@@ -7212,6 +7903,9 @@
       </c>
       <c r="E212" s="5" t="s">
         <v>290</v>
+      </c>
+      <c r="F212" s="11">
+        <v>40057</v>
       </c>
       <c r="G212" s="10"/>
       <c r="H212" s="10"/>
@@ -7248,7 +7942,7 @@
       <c r="AM212" s="10"/>
       <c r="AN212" s="10"/>
     </row>
-    <row r="213" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A213" s="10" t="s">
         <v>291</v>
       </c>
@@ -7268,7 +7962,7 @@
         <v>39661</v>
       </c>
     </row>
-    <row r="214" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
         <v>291</v>
       </c>
@@ -7283,6 +7977,9 @@
       </c>
       <c r="E214" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="F214" s="11">
+        <v>39661</v>
       </c>
       <c r="G214" s="10"/>
       <c r="H214" s="10"/>
@@ -7319,7 +8016,7 @@
       <c r="AM214" s="10"/>
       <c r="AN214" s="10"/>
     </row>
-    <row r="215" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A215" s="10" t="s">
         <v>294</v>
       </c>
@@ -7339,7 +8036,7 @@
         <v>39569</v>
       </c>
     </row>
-    <row r="216" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
         <v>294</v>
       </c>
@@ -7354,6 +8051,9 @@
       </c>
       <c r="E216" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="F216" s="11">
+        <v>39569</v>
       </c>
       <c r="G216" s="10"/>
       <c r="H216" s="10"/>
@@ -7390,7 +8090,7 @@
       <c r="AM216" s="10"/>
       <c r="AN216" s="10"/>
     </row>
-    <row r="217" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A217" s="10" t="s">
         <v>297</v>
       </c>
@@ -7410,7 +8110,7 @@
         <v>36739</v>
       </c>
     </row>
-    <row r="218" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="5" t="s">
         <v>297</v>
       </c>
@@ -7425,6 +8125,9 @@
       </c>
       <c r="E218" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="F218" s="11">
+        <v>36739</v>
       </c>
       <c r="G218" s="10"/>
       <c r="H218" s="10"/>
@@ -7461,7 +8164,7 @@
       <c r="AM218" s="10"/>
       <c r="AN218" s="10"/>
     </row>
-    <row r="219" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>300</v>
       </c>
@@ -7481,7 +8184,7 @@
         <v>38626</v>
       </c>
     </row>
-    <row r="220" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="5" t="s">
         <v>300</v>
       </c>
@@ -7497,8 +8200,11 @@
       <c r="E220" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="221" spans="1:40" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F220" s="4">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="221" spans="1:40" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>300</v>
       </c>
@@ -7518,7 +8224,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="222" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>300</v>
       </c>
@@ -7538,7 +8244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
         <v>300</v>
       </c>
@@ -7554,9 +8260,11 @@
       <c r="E223" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F223" s="5"/>
-    </row>
-    <row r="224" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="F223" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="224" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>300</v>
       </c>
@@ -7576,7 +8284,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="5" t="s">
         <v>307</v>
       </c>
@@ -7592,8 +8300,11 @@
       <c r="E225" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F225" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>307</v>
       </c>
@@ -7613,7 +8324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="5" t="s">
         <v>307</v>
       </c>
@@ -7629,9 +8340,11 @@
       <c r="E227" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F227" s="5"/>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F227" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>307</v>
       </c>
@@ -7651,7 +8364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>307</v>
       </c>
@@ -7667,9 +8380,11 @@
       <c r="E229" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F229" s="22"/>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F229" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="5" t="s">
         <v>307</v>
       </c>
@@ -7685,9 +8400,11 @@
       <c r="E230" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F230" s="5"/>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F230" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>314</v>
       </c>
@@ -7695,7 +8412,7 @@
         <v>52</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D231" s="22" t="s">
         <v>15</v>
@@ -7707,7 +8424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>314</v>
       </c>
@@ -7715,7 +8432,7 @@
         <v>52</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D232" s="27" t="s">
         <v>188</v>
@@ -7723,8 +8440,11 @@
       <c r="E232" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F232" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="8" t="s">
         <v>314</v>
       </c>
@@ -7732,7 +8452,7 @@
         <v>53</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D233" s="32" t="s">
         <v>15</v>
@@ -7744,7 +8464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="5" t="s">
         <v>314</v>
       </c>
@@ -7752,7 +8472,7 @@
         <v>53</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D234" s="31" t="s">
         <v>188</v>
@@ -7760,9 +8480,11 @@
       <c r="E234" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F234" s="5"/>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F234" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="8" t="s">
         <v>314</v>
       </c>
@@ -7770,7 +8492,7 @@
         <v>54</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D235" s="32" t="s">
         <v>15</v>
@@ -7782,7 +8504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="5" t="s">
         <v>314</v>
       </c>
@@ -7790,7 +8512,7 @@
         <v>54</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D236" s="31" t="s">
         <v>188</v>
@@ -7798,9 +8520,11 @@
       <c r="E236" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F236" s="5"/>
-    </row>
-    <row r="237" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F236" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="8" t="s">
         <v>314</v>
       </c>
@@ -7820,7 +8544,7 @@
         <v>38626</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="5" t="s">
         <v>314</v>
       </c>
@@ -7836,19 +8560,8 @@
       <c r="E238" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F238" s="5"/>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E240" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="F240" s="5" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="241" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F241" s="1" t="s">
-        <v>318</v>
+      <c r="F238" s="19">
+        <v>38626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>